<commit_message>
added APIs for subject and question
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Interview\project\online-exam-portal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{592DB286-E9DB-429D-892E-7C2F6DE31597}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F9928BC-7B61-4F2B-A991-38850E858224}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{2867269C-9739-4F59-806E-3FD917D80074}"/>
   </bookViews>
@@ -1844,7 +1844,7 @@
   <dimension ref="A1:Q24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2085,7 +2085,7 @@
         <v>4</v>
       </c>
       <c r="I7" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>

</xml_diff>